<commit_message>
Optimize API calls, add P/B and Profit Growth to Key Metrics, fix EPS display to use eps_ttm
</commit_message>
<xml_diff>
--- a/data/PNC.xlsx
+++ b/data/PNC.xlsx
@@ -73,7 +73,7 @@
     <t>Ngày xuất</t>
   </si>
   <si>
-    <t>17/12/2025</t>
+    <t>21/12/2025</t>
   </si>
   <si>
     <t>PNC</t>
@@ -5541,7 +5541,7 @@
         <v>4.670110661E10</v>
       </c>
       <c r="G38" s="13" t="n">
-        <v>3.3257715912E10</v>
+        <v>3.3257715911E10</v>
       </c>
       <c r="H38" s="13" t="n">
         <v>3.318446126E10</v>
@@ -9963,7 +9963,7 @@
         <v>1.576388957E9</v>
       </c>
       <c r="G71" s="13" t="n">
-        <v>1.478818646E9</v>
+        <v>1.478818645E9</v>
       </c>
       <c r="H71" s="13" t="n">
         <v>1.122116442E9</v>
@@ -10097,7 +10097,7 @@
         <v>8.64725998E8</v>
       </c>
       <c r="G72" s="13" t="n">
-        <v>9.33809983E8</v>
+        <v>9.33809982E8</v>
       </c>
       <c r="H72" s="13" t="n">
         <v>7.77566166E8</v>
@@ -10767,7 +10767,7 @@
         <v>5.1125743123E11</v>
       </c>
       <c r="G77" s="13" t="n">
-        <v>5.37822665037E11</v>
+        <v>5.37822665036E11</v>
       </c>
       <c r="H77" s="13" t="n">
         <v>5.27721953738E11</v>
@@ -14969,7 +14969,7 @@
         <v>1.52206327328E11</v>
       </c>
       <c r="G109" s="13" t="n">
-        <v>1.65463825279E11</v>
+        <v>1.65463825278E11</v>
       </c>
       <c r="H109" s="13" t="n">
         <v>1.82243725671E11</v>
@@ -15103,7 +15103,7 @@
         <v>1.52206327328E11</v>
       </c>
       <c r="G110" s="13" t="n">
-        <v>1.65463825279E11</v>
+        <v>1.65463825278E11</v>
       </c>
       <c r="H110" s="13" t="n">
         <v>1.82243725671E11</v>
@@ -15377,7 +15377,7 @@
         <v>1.1040241E11</v>
       </c>
       <c r="I112" s="13" t="n">
-        <v>1.040241E10</v>
+        <v>1.1040241E11</v>
       </c>
       <c r="K112" s="13" t="n">
         <v>1.1040241E11</v>
@@ -16979,7 +16979,7 @@
         <v>1.7682724208E10</v>
       </c>
       <c r="G124" s="13" t="n">
-        <v>3.0940222159E10</v>
+        <v>3.0940222158E10</v>
       </c>
       <c r="H124" s="13" t="n">
         <v>4.7720122551E10</v>
@@ -17113,10 +17113,10 @@
         <v>3.2742256781E10</v>
       </c>
       <c r="G125" s="13" t="n">
-        <v>1.7682724208E10</v>
+        <v>3.0940222158E10</v>
       </c>
       <c r="H125" s="13" t="n">
-        <v>3.0940222158E10</v>
+        <v>4.7720122551E10</v>
       </c>
       <c r="I125" s="13" t="n">
         <v>4.2320447051E10</v>
@@ -17247,10 +17247,10 @@
         <v>-1.5059532573E10</v>
       </c>
       <c r="G126" s="13" t="n">
-        <v>1.3257497951E10</v>
+        <v>0.0</v>
       </c>
       <c r="H126" s="13" t="n">
-        <v>1.6779900393E10</v>
+        <v>0.0</v>
       </c>
       <c r="I126" s="13" t="n">
         <v>1.0213532598E10</v>
@@ -18185,7 +18185,7 @@
         <v>5.1125743123E11</v>
       </c>
       <c r="G133" s="13" t="n">
-        <v>5.37822665037E11</v>
+        <v>5.37822665036E11</v>
       </c>
       <c r="H133" s="13" t="n">
         <v>5.27721953738E11</v>
@@ -22639,7 +22639,7 @@
         <v>2.7140739E8</v>
       </c>
       <c r="G15" s="21" t="n">
-        <v>1.5739279102E10</v>
+        <v>1.5739279103E10</v>
       </c>
       <c r="H15" s="21" t="n">
         <v>2.710072319E9</v>
@@ -23443,7 +23443,7 @@
         <v>0.0</v>
       </c>
       <c r="G21" s="21" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="H21" s="21" t="n">
         <v>0.0</v>

</xml_diff>